<commit_message>
Refactoring 10/29/24 @ 22:14
</commit_message>
<xml_diff>
--- a/data/Auth.xlsx
+++ b/data/Auth.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -27,10 +27,38 @@
     <t>Excel Worksheet Name</t>
   </si>
   <si>
+    <t>Export Summary</t>
+  </si>
+  <si>
+    <t>Table 1</t>
+  </si>
+  <si>
     <t>Auth</t>
   </si>
   <si>
-    <t>Table 1</t>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="11"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Auth</t>
+    </r>
+  </si>
+  <si>
+    <t>Auth-Front</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="11"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Auth-Front</t>
+    </r>
   </si>
   <si>
     <t>email</t>
@@ -63,7 +91,7 @@
     <t>useragent</t>
   </si>
   <si>
-    <t>Auth-Front</t>
+    <t>123.456.7890</t>
   </si>
 </sst>
 </file>
@@ -142,7 +170,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="12"/>
+        <fgColor indexed="13"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -157,11 +185,20 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="12"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -169,57 +206,20 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </right>
       <top style="thin">
-        <color indexed="13"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top style="thin">
-        <color indexed="13"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top style="thin">
-        <color indexed="13"/>
-      </top>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right/>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -233,7 +233,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </right>
       <top/>
       <bottom/>
@@ -241,12 +241,12 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </bottom>
       <diagonal/>
     </border>
@@ -255,18 +255,46 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="12"/>
       </bottom>
       <diagonal/>
     </border>
@@ -276,7 +304,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -298,36 +326,99 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="49" fontId="6" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -343,16 +434,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -375,8 +463,8 @@
       <rgbColor rgb="ff5e88b1"/>
       <rgbColor rgb="ffeef3f4"/>
       <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ff0451a5"/>
       <rgbColor rgb="ff1f1f1f"/>
     </indexedColors>
@@ -1410,73 +1498,162 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
+    <col min="1" max="1" width="2" style="6" customWidth="1"/>
     <col min="2" max="4" width="33.6016" customWidth="1"/>
+    <col min="2" max="2" width="33.6719" style="6" customWidth="1"/>
+    <col min="3" max="3" width="33.6719" style="6" customWidth="1"/>
+    <col min="4" max="4" width="33.6719" style="6" customWidth="1"/>
+    <col min="5" max="5" width="10" style="6" customWidth="1"/>
+    <col min="6" max="16384" width="10" style="6" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" ht="13.65" customHeight="1">
+      <c r="A1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="9"/>
+    </row>
+    <row r="2" ht="13.65" customHeight="1">
+      <c r="A2" s="10"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="12"/>
+    </row>
     <row r="3" ht="50" customHeight="1">
-      <c r="B3" t="s" s="1">
+      <c r="A3" s="10"/>
+      <c r="B3" t="s" s="13">
         <v>0</v>
       </c>
-      <c r="C3"/>
-      <c r="D3"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="12"/>
+    </row>
+    <row r="4" ht="13.65" customHeight="1">
+      <c r="A4" s="10"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="12"/>
+    </row>
+    <row r="5" ht="13.65" customHeight="1">
+      <c r="A5" s="10"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="12"/>
+    </row>
+    <row r="6" ht="13.65" customHeight="1">
+      <c r="A6" s="10"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="12"/>
     </row>
     <row r="7">
-      <c r="B7" t="s" s="2">
+      <c r="A7" s="10"/>
+      <c r="B7" t="s" s="14">
         <v>1</v>
       </c>
-      <c r="C7" t="s" s="2">
+      <c r="C7" t="s" s="14">
         <v>2</v>
       </c>
-      <c r="D7" t="s" s="2">
+      <c r="D7" t="s" s="14">
         <v>3</v>
       </c>
+      <c r="E7" s="12"/>
+    </row>
+    <row r="8" ht="13.65" customHeight="1">
+      <c r="A8" s="10"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="12"/>
     </row>
     <row r="9">
-      <c r="B9" t="s" s="3">
-        <v>4</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="A9" s="10"/>
+      <c r="B9" t="s" s="15">
+        <v>6</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="12"/>
     </row>
     <row r="10">
-      <c r="B10" s="4"/>
-      <c r="C10" t="s" s="4">
+      <c r="A10" s="10"/>
+      <c r="B10" s="17"/>
+      <c r="C10" t="s" s="18">
         <v>5</v>
       </c>
-      <c r="D10" t="s" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11">
+      <c r="D10" t="s" s="19">
+        <v>7</v>
+      </c>
+      <c r="E10" s="12"/>
+    </row>
+    <row r="11" ht="13" customHeight="1">
+      <c r="A11" s="10"/>
       <c r="B11" t="s" s="3">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-    </row>
-    <row r="12">
+      <c r="E11" s="12"/>
+    </row>
+    <row r="12" ht="13" customHeight="1">
+      <c r="A12" s="20"/>
       <c r="B12" s="4"/>
       <c r="C12" t="s" s="4">
         <v>5</v>
       </c>
       <c r="D12" t="s" s="5">
-        <v>16</v>
+        <v>6</v>
+      </c>
+      <c r="E12" s="24"/>
+    </row>
+    <row r="13">
+      <c r="B13" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14">
+      <c r="B14" s="4"/>
+      <c r="C14" t="s" s="4">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s" s="5">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
+    <mergeCell ref="B3:D3"/>
     <mergeCell ref="B3:D3"/>
   </mergeCells>
   <hyperlinks>
+    <hyperlink ref="D10" location="'Export Summary'!R1C1" tooltip="" display="Export Summary"/>
     <hyperlink ref="D10" location="'Auth'!R1C1" tooltip="" display="Auth"/>
     <hyperlink ref="D12" location="'Auth-Front'!R1C1" tooltip="" display="Auth-Front"/>
+    <hyperlink ref="D12" location="'Auth'!R1C1" tooltip="" display="Auth"/>
+    <hyperlink ref="D14" location="'Auth-Front'!R1C1" tooltip="" display="Auth-Front"/>
   </hyperlinks>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -1491,127 +1668,127 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6667" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="7" width="12.6719" style="6" customWidth="1"/>
-    <col min="8" max="16384" width="12.6719" style="6" customWidth="1"/>
+    <col min="1" max="7" width="12.6719" style="25" customWidth="1"/>
+    <col min="8" max="16384" width="12.6719" style="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1">
-      <c r="A1" t="s" s="7">
-        <v>6</v>
-      </c>
-      <c r="B1" t="s" s="8">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s" s="9">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s" s="9">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s" s="9">
+      <c r="A1" t="s" s="26">
         <v>10</v>
       </c>
-      <c r="F1" t="s" s="10">
+      <c r="B1" t="s" s="27">
         <v>11</v>
       </c>
-      <c r="G1" t="s" s="9">
+      <c r="C1" t="s" s="28">
         <v>12</v>
       </c>
+      <c r="D1" t="s" s="28">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s" s="28">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s" s="29">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s" s="28">
+        <v>16</v>
+      </c>
     </row>
     <row r="2" ht="15" customHeight="1">
-      <c r="A2" t="s" s="11">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s" s="12">
+      <c r="A2" t="s" s="30">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s" s="31">
+        <v>18</v>
+      </c>
+      <c r="C2" s="32">
+        <v>123.4567</v>
+      </c>
+      <c r="D2" s="33">
+        <v>123.4567</v>
+      </c>
+      <c r="E2" t="s" s="34">
         <v>14</v>
       </c>
-      <c r="C2" s="13">
-        <v>1234567</v>
-      </c>
-      <c r="D2" s="14">
-        <v>1234567</v>
-      </c>
-      <c r="E2" t="s" s="15">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s" s="9">
-        <v>15</v>
-      </c>
-      <c r="G2" t="s" s="15">
-        <v>12</v>
+      <c r="F2" t="s" s="28">
+        <v>19</v>
+      </c>
+      <c r="G2" t="s" s="34">
+        <v>20</v>
       </c>
     </row>
     <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" s="16"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="18"/>
+      <c r="A3" s="35"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="37"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="16"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="20"/>
+      <c r="A4" s="35"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="39"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="16"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="20"/>
+      <c r="A5" s="35"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="39"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="16"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="20"/>
+      <c r="A6" s="35"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="39"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="16"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="20"/>
+      <c r="A7" s="35"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="39"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="16"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="20"/>
+      <c r="A8" s="35"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="39"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="16"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="20"/>
+      <c r="A9" s="35"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="39"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="21"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="23"/>
+      <c r="A10" s="40"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="42"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
@@ -1627,31 +1804,93 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6667" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="2" width="12.6719" style="24" customWidth="1"/>
-    <col min="3" max="16384" width="12.6719" style="24" customWidth="1"/>
+    <col min="1" max="5" width="12.6719" style="43" customWidth="1"/>
+    <col min="6" max="16384" width="12.6719" style="43" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1">
-      <c r="A1" t="s" s="7">
-        <v>6</v>
-      </c>
-      <c r="B1" t="s" s="8">
-        <v>7</v>
-      </c>
+      <c r="A1" t="s" s="26">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s" s="27">
+        <v>11</v>
+      </c>
+      <c r="C1" s="44"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="37"/>
     </row>
     <row r="2" ht="15" customHeight="1">
-      <c r="A2" t="s" s="25">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s" s="12">
-        <v>14</v>
-      </c>
+      <c r="A2" t="s" s="45">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s" s="31">
+        <v>18</v>
+      </c>
+      <c r="C2" s="35"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="39"/>
+    </row>
+    <row r="3" ht="13.65" customHeight="1">
+      <c r="A3" s="44"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="39"/>
+    </row>
+    <row r="4" ht="13.65" customHeight="1">
+      <c r="A4" s="35"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="39"/>
+    </row>
+    <row r="5" ht="13.65" customHeight="1">
+      <c r="A5" s="35"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="39"/>
+    </row>
+    <row r="6" ht="13.65" customHeight="1">
+      <c r="A6" s="35"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="39"/>
+    </row>
+    <row r="7" ht="13.65" customHeight="1">
+      <c r="A7" s="35"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="39"/>
+    </row>
+    <row r="8" ht="13.65" customHeight="1">
+      <c r="A8" s="35"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="39"/>
+    </row>
+    <row r="9" ht="13.65" customHeight="1">
+      <c r="A9" s="35"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="39"/>
+    </row>
+    <row r="10" ht="13.65" customHeight="1">
+      <c r="A10" s="40"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="42"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>